<commit_message>
Client에 Kingdom api 추가.
TODO: Buy api 사용시  Arithmetic operation resulted in an overflow 오류
</commit_message>
<xml_diff>
--- a/Data/Excel/Model/User/KingdomStructure.xlsx
+++ b/Data/Excel/Model/User/KingdomStructure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Model\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431AD609-2D35-4853-9911-CE1D4106ECED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD57792-B7C5-482B-B488-1415E4090B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -1036,17 +1036,17 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="3" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="3" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1066,21 +1066,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1094,7 +1091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1113,7 +1110,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1121,7 +1118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>

</xml_diff>